<commit_message>
Some extra gfx labels, and offset label - known issue with data insertion (compiled size is wrong) to find/fix
</commit_message>
<xml_diff>
--- a/segments.xlsx
+++ b/segments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom.cresswell/Dropbox/Geek/Gaming Projects/Bloodwych 68k/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4B1273-204B-7941-8973-6821476E3E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A19D8-A467-884D-8E3E-38735BC16714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="880" windowWidth="32720" windowHeight="22140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9140" yWindow="880" windowWidth="32720" windowHeight="22140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOODWYCH439" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5765" uniqueCount="3409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5765" uniqueCount="3419">
   <si>
     <t>Type</t>
   </si>
@@ -9473,9 +9473,6 @@
     <t>_Offset_AudioSampleOffsets_0x2</t>
   </si>
   <si>
-    <t>_Offset_PocketContents_0x02</t>
-  </si>
-  <si>
     <t>_Delete</t>
   </si>
   <si>
@@ -9692,12 +9689,6 @@
     <t>Switches.colours</t>
   </si>
   <si>
-    <t>_Offset_CharacterStats_0x11</t>
-  </si>
-  <si>
-    <t>_Offset_CharacterStats_0x05</t>
-  </si>
-  <si>
     <t>_Offset_CurrentTower_0x01</t>
   </si>
   <si>
@@ -10199,9 +10190,6 @@
     <t>$481FC</t>
   </si>
   <si>
-    <t>_Offset_CharacterStats_0x80</t>
-  </si>
-  <si>
     <t>Door_Lock_Colours</t>
   </si>
   <si>
@@ -10263,6 +10251,48 @@
   </si>
   <si>
     <t>GFX_CrabFace_Position</t>
+  </si>
+  <si>
+    <t>Draw_Pillar</t>
+  </si>
+  <si>
+    <t>_Offset_Character_Stats_DataTable_0x05</t>
+  </si>
+  <si>
+    <t>_Offset_Character_Stats_DataTable_0x11</t>
+  </si>
+  <si>
+    <t>_Offset_Character_Stats_DataTable_0x80</t>
+  </si>
+  <si>
+    <t>_Offset_Character_Pockets_DataTable_0x02</t>
+  </si>
+  <si>
+    <t>Flip_Sprite</t>
+  </si>
+  <si>
+    <t>Draw_Wall_Sprite</t>
+  </si>
+  <si>
+    <t>GFX_Misc_Pillar_SpriteTable</t>
+  </si>
+  <si>
+    <t>GFX_Main_Wall_SpriteTable</t>
+  </si>
+  <si>
+    <t>Bitplane_Mask</t>
+  </si>
+  <si>
+    <t>Draw_Main_Shelf_Overlay</t>
+  </si>
+  <si>
+    <t>Draw_Main_Object_Overlay</t>
+  </si>
+  <si>
+    <t>Draw_Main_Sign_Overlay</t>
+  </si>
+  <si>
+    <t>Draw_Main_Switch_Overlay</t>
   </si>
 </sst>
 </file>
@@ -10817,8 +10847,8 @@
   <dimension ref="A1:T2644"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A2001" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2044" sqref="E2044"/>
+      <pane ySplit="3" topLeftCell="A2187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2216" sqref="D2216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11364,13 +11394,13 @@
         <v>1759</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>3240</v>
+        <v>3237</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>3239</v>
+        <v>3236</v>
       </c>
       <c r="E16" s="19" t="str">
         <f t="shared" si="0"/>
@@ -11396,7 +11426,7 @@
         <v>1760</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>3241</v>
+        <v>3238</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>8</v>
@@ -11409,7 +11439,7 @@
         <v>maps/keep.entrances</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>3243</v>
+        <v>3240</v>
       </c>
       <c r="G17" s="18">
         <f t="shared" si="1"/>
@@ -11428,7 +11458,7 @@
         <v>1770</v>
       </c>
       <c r="B18" t="s">
-        <v>3242</v>
+        <v>3239</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>48</v>
@@ -11460,13 +11490,13 @@
         <v>2282</v>
       </c>
       <c r="B19" t="s">
-        <v>3293</v>
+        <v>3290</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>3303</v>
+        <v>3300</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -11492,13 +11522,13 @@
         <v>2283</v>
       </c>
       <c r="B20" t="s">
-        <v>3292</v>
+        <v>3289</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>51</v>
       </c>
       <c r="D20" t="s">
-        <v>3302</v>
+        <v>3299</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="0"/>
@@ -11524,7 +11554,7 @@
         <v>2294</v>
       </c>
       <c r="B21" t="s">
-        <v>3294</v>
+        <v>3291</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>51</v>
@@ -11556,7 +11586,7 @@
         <v>2347</v>
       </c>
       <c r="B22" t="s">
-        <v>3295</v>
+        <v>3292</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>51</v>
@@ -11588,7 +11618,7 @@
         <v>3129</v>
       </c>
       <c r="B23" t="s">
-        <v>3296</v>
+        <v>3293</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>51</v>
@@ -11601,7 +11631,7 @@
         <v>monsters/summon.colours</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>3249</v>
+        <v>3246</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="1"/>
@@ -11620,7 +11650,7 @@
         <v>2383</v>
       </c>
       <c r="B24" t="s">
-        <v>3297</v>
+        <v>3294</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>51</v>
@@ -11633,7 +11663,7 @@
         <v>monsters/dragon.colours</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>3250</v>
+        <v>3247</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" si="1"/>
@@ -11652,7 +11682,7 @@
         <v>2404</v>
       </c>
       <c r="B25" t="s">
-        <v>3298</v>
+        <v>3295</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>51</v>
@@ -11665,7 +11695,7 @@
         <v>monsters/behemoth.colours</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>3251</v>
+        <v>3248</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" si="1"/>
@@ -11729,7 +11759,7 @@
         <v>data/characters.heads</v>
       </c>
       <c r="F27" t="s">
-        <v>3254</v>
+        <v>3251</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="1"/>
@@ -11748,7 +11778,7 @@
         <v>2921</v>
       </c>
       <c r="B28" s="22" t="s">
-        <v>3333</v>
+        <v>3330</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>48</v>
@@ -11780,7 +11810,7 @@
         <v>2922</v>
       </c>
       <c r="B29" t="s">
-        <v>3332</v>
+        <v>3329</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>48</v>
@@ -11812,7 +11842,7 @@
         <v>2916</v>
       </c>
       <c r="B30" t="s">
-        <v>3290</v>
+        <v>3287</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>48</v>
@@ -11844,20 +11874,20 @@
         <v>2924</v>
       </c>
       <c r="B31" t="s">
-        <v>3299</v>
+        <v>3296</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D31" t="s">
-        <v>3291</v>
+        <v>3288</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
         <v>data/objectfloor.colours</v>
       </c>
       <c r="F31" t="s">
-        <v>3337</v>
+        <v>3334</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" si="1"/>
@@ -11876,20 +11906,20 @@
         <v>2925</v>
       </c>
       <c r="B32" t="s">
-        <v>3300</v>
+        <v>3297</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D32" t="s">
-        <v>3301</v>
+        <v>3298</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
         <v>data/objectfloor.palette</v>
       </c>
       <c r="F32" t="s">
-        <v>3336</v>
+        <v>3333</v>
       </c>
       <c r="G32" s="5">
         <f t="shared" si="1"/>
@@ -11921,7 +11951,7 @@
         <v>gfx/ObjectsOnFloor.gfx</v>
       </c>
       <c r="F33" t="s">
-        <v>3252</v>
+        <v>3249</v>
       </c>
       <c r="G33" s="5">
         <f>IF(F33&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F33,"adrEA",""),"$","")),"")</f>
@@ -11940,7 +11970,7 @@
         <v>2926</v>
       </c>
       <c r="B34" t="s">
-        <v>3234</v>
+        <v>3231</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>124</v>
@@ -11953,7 +11983,7 @@
         <v>gfx/ObjectsOnFloor.offsets</v>
       </c>
       <c r="F34" t="s">
-        <v>3335</v>
+        <v>3332</v>
       </c>
       <c r="G34" s="5">
         <f>IF(F34&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F34,"adrEA",""),"$","")),"")</f>
@@ -11972,7 +12002,7 @@
         <v>2923</v>
       </c>
       <c r="B35" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>124</v>
@@ -11985,7 +12015,7 @@
         <v>gfx/ObjectsOnFloor.heights</v>
       </c>
       <c r="F35" t="s">
-        <v>3334</v>
+        <v>3331</v>
       </c>
       <c r="G35" s="5">
         <f>IF(F35&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F35,"adrEA",""),"$","")),"")</f>
@@ -12009,7 +12039,7 @@
         <v>2940</v>
       </c>
       <c r="B37" t="s">
-        <v>3392</v>
+        <v>3388</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>48</v>
@@ -12041,7 +12071,7 @@
         <v>2944</v>
       </c>
       <c r="B38" t="s">
-        <v>3393</v>
+        <v>3389</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>48</v>
@@ -12073,7 +12103,7 @@
         <v>3055</v>
       </c>
       <c r="B39" t="s">
-        <v>3246</v>
+        <v>3243</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>48</v>
@@ -12105,7 +12135,7 @@
         <v>3054</v>
       </c>
       <c r="B40" t="s">
-        <v>3245</v>
+        <v>3242</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>48</v>
@@ -12137,20 +12167,20 @@
         <v>1434</v>
       </c>
       <c r="B41" t="s">
-        <v>3244</v>
+        <v>3241</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D41" t="s">
-        <v>3247</v>
+        <v>3244</v>
       </c>
       <c r="E41" t="str">
         <f>C41&amp;"/"&amp;D41</f>
         <v>data/scrollstowers.data</v>
       </c>
       <c r="F41" t="s">
-        <v>3248</v>
+        <v>3245</v>
       </c>
       <c r="G41" s="5">
         <f t="shared" si="1"/>
@@ -12294,7 +12324,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>3399</v>
+        <v>3395</v>
       </c>
       <c r="B46" t="s">
         <v>3128</v>
@@ -12550,7 +12580,7 @@
     </row>
     <row r="54" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B54" s="12" t="s">
         <v>3030</v>
@@ -12582,7 +12612,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="5" t="s">
@@ -12612,7 +12642,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="5" t="s">
@@ -12642,7 +12672,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="5" t="s">
@@ -12672,7 +12702,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="5" t="s">
@@ -12702,7 +12732,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="5" t="s">
@@ -12732,7 +12762,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="5" t="s">
@@ -12792,7 +12822,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="5" t="s">
@@ -12822,7 +12852,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="5" t="s">
@@ -12852,7 +12882,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="5" t="s">
@@ -12882,7 +12912,7 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B65" s="9"/>
       <c r="C65" s="5" t="s">
@@ -12912,7 +12942,7 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="12" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="B66" s="9"/>
       <c r="C66" s="5" t="s">
@@ -12989,7 +13019,7 @@
         <v>3044</v>
       </c>
       <c r="B68" t="s">
-        <v>3228</v>
+        <v>3225</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>124</v>
@@ -13002,7 +13032,7 @@
         <v>gfx/ButtonHighlights.gfx</v>
       </c>
       <c r="F68" t="s">
-        <v>3256</v>
+        <v>3253</v>
       </c>
       <c r="G68" s="5">
         <f>IF(F68&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F68,"adrEA",""),"$","")),"")</f>
@@ -13032,7 +13062,7 @@
         <v>18B7A</v>
       </c>
       <c r="O68" t="s">
-        <v>3255</v>
+        <v>3252</v>
       </c>
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
@@ -13040,7 +13070,7 @@
         <v>3045</v>
       </c>
       <c r="B69" t="s">
-        <v>3229</v>
+        <v>3226</v>
       </c>
       <c r="C69" s="5" t="s">
         <v>124</v>
@@ -13053,7 +13083,7 @@
         <v>gfx/Scroll_Edge_Top.gfx</v>
       </c>
       <c r="F69" t="s">
-        <v>3257</v>
+        <v>3254</v>
       </c>
       <c r="G69" s="5">
         <f>IF(F69&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F69,"adrEA",""),"$","")),"")</f>
@@ -13088,7 +13118,7 @@
         <v>3046</v>
       </c>
       <c r="B70" t="s">
-        <v>3231</v>
+        <v>3228</v>
       </c>
       <c r="C70" s="5" t="s">
         <v>124</v>
@@ -13101,7 +13131,7 @@
         <v>gfx/Scroll_Edge_Bottom.gfx</v>
       </c>
       <c r="F70" t="s">
-        <v>3258</v>
+        <v>3255</v>
       </c>
       <c r="G70" s="5">
         <f>IF(F70&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F70,"adrEA",""),"$","")),"")</f>
@@ -13136,7 +13166,7 @@
         <v>3047</v>
       </c>
       <c r="B71" t="s">
-        <v>3230</v>
+        <v>3227</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>124</v>
@@ -13149,7 +13179,7 @@
         <v>gfx/Scroll_Edge_Left.gfx</v>
       </c>
       <c r="F71" t="s">
-        <v>3259</v>
+        <v>3256</v>
       </c>
       <c r="G71" s="5">
         <f>IF(F71&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F71,"adrEA",""),"$","")),"")</f>
@@ -13184,7 +13214,7 @@
         <v>3048</v>
       </c>
       <c r="B72" t="s">
-        <v>3232</v>
+        <v>3229</v>
       </c>
       <c r="C72" s="5" t="s">
         <v>124</v>
@@ -13197,7 +13227,7 @@
         <v>gfx/Scroll_Edge_Right.gfx</v>
       </c>
       <c r="F72" t="s">
-        <v>3260</v>
+        <v>3257</v>
       </c>
       <c r="G72" s="5">
         <f>G71+H71</f>
@@ -13232,7 +13262,7 @@
         <v>3049</v>
       </c>
       <c r="B73" t="s">
-        <v>3233</v>
+        <v>3230</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>124</v>
@@ -13245,7 +13275,7 @@
         <v>gfx/Shield_Clicked.gfx</v>
       </c>
       <c r="F73" t="s">
-        <v>3261</v>
+        <v>3258</v>
       </c>
       <c r="G73" s="5">
         <f>G72+H72</f>
@@ -13280,7 +13310,7 @@
         <v>3056</v>
       </c>
       <c r="B74" t="s">
-        <v>3192</v>
+        <v>3191</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>124</v>
@@ -13320,7 +13350,7 @@
         <v>3057</v>
       </c>
       <c r="B75" t="s">
-        <v>3215</v>
+        <v>3214</v>
       </c>
       <c r="C75" s="5" t="s">
         <v>124</v>
@@ -13352,7 +13382,7 @@
         <v>3058</v>
       </c>
       <c r="B76" t="s">
-        <v>3193</v>
+        <v>3192</v>
       </c>
       <c r="C76" s="5" t="s">
         <v>124</v>
@@ -13384,7 +13414,7 @@
         <v>3059</v>
       </c>
       <c r="B77" t="s">
-        <v>3201</v>
+        <v>3200</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>124</v>
@@ -13416,7 +13446,7 @@
         <v>3060</v>
       </c>
       <c r="B78" t="s">
-        <v>3202</v>
+        <v>3201</v>
       </c>
       <c r="C78" s="5" t="s">
         <v>124</v>
@@ -13448,7 +13478,7 @@
         <v>3061</v>
       </c>
       <c r="B79" t="s">
-        <v>3203</v>
+        <v>3202</v>
       </c>
       <c r="C79" s="5" t="s">
         <v>124</v>
@@ -13480,7 +13510,7 @@
         <v>3062</v>
       </c>
       <c r="B80" t="s">
-        <v>3204</v>
+        <v>3203</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>124</v>
@@ -13512,7 +13542,7 @@
         <v>3063</v>
       </c>
       <c r="B81" t="s">
-        <v>3205</v>
+        <v>3204</v>
       </c>
       <c r="C81" s="5" t="s">
         <v>124</v>
@@ -13544,7 +13574,7 @@
         <v>3064</v>
       </c>
       <c r="B82" t="s">
-        <v>3206</v>
+        <v>3205</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>124</v>
@@ -13576,7 +13606,7 @@
         <v>3065</v>
       </c>
       <c r="B83" t="s">
-        <v>3207</v>
+        <v>3206</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>124</v>
@@ -13608,7 +13638,7 @@
         <v>3066</v>
       </c>
       <c r="B84" t="s">
-        <v>3208</v>
+        <v>3207</v>
       </c>
       <c r="C84" s="5" t="s">
         <v>124</v>
@@ -13621,7 +13651,7 @@
         <v>gfx/Stairs_Up.gfx</v>
       </c>
       <c r="F84" t="s">
-        <v>3264</v>
+        <v>3261</v>
       </c>
       <c r="G84" s="5">
         <f t="shared" si="13"/>
@@ -13635,7 +13665,7 @@
         <v>1EA8</v>
       </c>
       <c r="L84" s="20" t="s">
-        <v>3263</v>
+        <v>3260</v>
       </c>
       <c r="M84">
         <f>HEX2DEC(L84)</f>
@@ -13647,7 +13677,7 @@
         <v>3067</v>
       </c>
       <c r="B85" t="s">
-        <v>3209</v>
+        <v>3208</v>
       </c>
       <c r="C85" s="5" t="s">
         <v>124</v>
@@ -13678,7 +13708,7 @@
         <v>2A7B4</v>
       </c>
       <c r="L85" t="s">
-        <v>3262</v>
+        <v>3259</v>
       </c>
       <c r="M85">
         <f>HEX2DEC(L85)</f>
@@ -13694,7 +13724,7 @@
         <v>3068</v>
       </c>
       <c r="B86" t="s">
-        <v>3210</v>
+        <v>3209</v>
       </c>
       <c r="C86" s="5" t="s">
         <v>124</v>
@@ -13726,7 +13756,7 @@
         <v>3069</v>
       </c>
       <c r="B87" t="s">
-        <v>3211</v>
+        <v>3210</v>
       </c>
       <c r="C87" s="5" t="s">
         <v>124</v>
@@ -13758,7 +13788,7 @@
         <v>3070</v>
       </c>
       <c r="B88" t="s">
-        <v>3212</v>
+        <v>3211</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>124</v>
@@ -13790,7 +13820,7 @@
         <v>3071</v>
       </c>
       <c r="B89" t="s">
-        <v>3213</v>
+        <v>3212</v>
       </c>
       <c r="C89" s="5" t="s">
         <v>124</v>
@@ -13803,7 +13833,7 @@
         <v>gfx/Pad_Pit_Low.gfx</v>
       </c>
       <c r="F89" t="s">
-        <v>3340</v>
+        <v>3337</v>
       </c>
       <c r="G89" s="5">
         <f t="shared" si="13"/>
@@ -13822,7 +13852,7 @@
         <v>3072</v>
       </c>
       <c r="B90" t="s">
-        <v>3214</v>
+        <v>3213</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>124</v>
@@ -13835,7 +13865,7 @@
         <v>gfx/Pad_Pit_High.gfx</v>
       </c>
       <c r="F90" t="s">
-        <v>3341</v>
+        <v>3338</v>
       </c>
       <c r="G90" s="5">
         <f t="shared" si="13"/>
@@ -13854,7 +13884,7 @@
         <v>3073</v>
       </c>
       <c r="B91" t="s">
-        <v>3200</v>
+        <v>3199</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>124</v>
@@ -13867,7 +13897,7 @@
         <v>gfx/Pad_Trigger.gfx</v>
       </c>
       <c r="F91" t="s">
-        <v>3342</v>
+        <v>3339</v>
       </c>
       <c r="G91" s="5">
         <f t="shared" si="13"/>
@@ -13899,7 +13929,7 @@
         <v>gfx/FloorCeiling.gfx</v>
       </c>
       <c r="F92" t="s">
-        <v>3253</v>
+        <v>3250</v>
       </c>
       <c r="G92" s="5">
         <f t="shared" si="13"/>
@@ -13931,7 +13961,7 @@
         <v>gfx/AirbourneFireball.gfx</v>
       </c>
       <c r="F93" t="s">
-        <v>3343</v>
+        <v>3340</v>
       </c>
       <c r="G93" s="5">
         <f t="shared" si="13"/>
@@ -13963,7 +13993,7 @@
         <v>gfx/AirbourneSpells.gfx</v>
       </c>
       <c r="F94" t="s">
-        <v>3344</v>
+        <v>3341</v>
       </c>
       <c r="G94" s="5">
         <f t="shared" si="13"/>
@@ -13995,7 +14025,7 @@
         <v>data/characters.colours</v>
       </c>
       <c r="F95" t="s">
-        <v>3345</v>
+        <v>3342</v>
       </c>
       <c r="G95" s="5">
         <f t="shared" si="13"/>
@@ -14014,7 +14044,7 @@
         <v>3080</v>
       </c>
       <c r="B96" t="s">
-        <v>3156</v>
+        <v>3155</v>
       </c>
       <c r="C96" s="5" t="s">
         <v>124</v>
@@ -14027,7 +14057,7 @@
         <v>gfx/HeadParts.gfx</v>
       </c>
       <c r="F96" t="s">
-        <v>3346</v>
+        <v>3343</v>
       </c>
       <c r="G96" s="5">
         <f t="shared" si="13"/>
@@ -14046,7 +14076,7 @@
         <v>3081</v>
       </c>
       <c r="B97" t="s">
-        <v>3199</v>
+        <v>3198</v>
       </c>
       <c r="C97" s="5" t="s">
         <v>124</v>
@@ -14059,7 +14089,7 @@
         <v>gfx/BodyParts.gfx</v>
       </c>
       <c r="F97" t="s">
-        <v>3347</v>
+        <v>3344</v>
       </c>
       <c r="G97" s="5">
         <f t="shared" si="13"/>
@@ -14078,20 +14108,20 @@
         <v>3083</v>
       </c>
       <c r="B98" t="s">
-        <v>3198</v>
+        <v>3197</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>124</v>
       </c>
       <c r="D98" t="s">
-        <v>3186</v>
+        <v>3185</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="12"/>
         <v>gfx/Avatars_Large.gfx</v>
       </c>
       <c r="F98" t="s">
-        <v>3348</v>
+        <v>3345</v>
       </c>
       <c r="G98" s="5">
         <f t="shared" si="13"/>
@@ -14110,7 +14140,7 @@
         <v>3084</v>
       </c>
       <c r="B99" t="s">
-        <v>3197</v>
+        <v>3196</v>
       </c>
       <c r="C99" s="5" t="s">
         <v>124</v>
@@ -14123,7 +14153,7 @@
         <v>gfx/Shield_Avatars.gfx</v>
       </c>
       <c r="F99" t="s">
-        <v>3349</v>
+        <v>3346</v>
       </c>
       <c r="G99" s="5">
         <f t="shared" si="13"/>
@@ -14142,7 +14172,7 @@
         <v>3085</v>
       </c>
       <c r="B100" t="s">
-        <v>3196</v>
+        <v>3195</v>
       </c>
       <c r="C100" s="5" t="s">
         <v>124</v>
@@ -14155,7 +14185,7 @@
         <v>gfx/ShieldTop.gfx</v>
       </c>
       <c r="F100" t="s">
-        <v>3350</v>
+        <v>3347</v>
       </c>
       <c r="G100" s="5">
         <f t="shared" si="13"/>
@@ -14174,7 +14204,7 @@
         <v>3086</v>
       </c>
       <c r="B101" t="s">
-        <v>3195</v>
+        <v>3194</v>
       </c>
       <c r="C101" s="5" t="s">
         <v>124</v>
@@ -14187,7 +14217,7 @@
         <v>gfx/ShieldBottom.gfx</v>
       </c>
       <c r="F101" t="s">
-        <v>3351</v>
+        <v>3348</v>
       </c>
       <c r="G101" s="5">
         <f t="shared" si="13"/>
@@ -14206,7 +14236,7 @@
         <v>3087</v>
       </c>
       <c r="B102" t="s">
-        <v>3194</v>
+        <v>3193</v>
       </c>
       <c r="C102" s="5" t="s">
         <v>124</v>
@@ -14219,7 +14249,7 @@
         <v>gfx/ShieldClasses.gfx</v>
       </c>
       <c r="F102" t="s">
-        <v>3352</v>
+        <v>3349</v>
       </c>
       <c r="G102" s="5">
         <f t="shared" si="13"/>
@@ -14238,7 +14268,7 @@
         <v>3088</v>
       </c>
       <c r="B103" t="s">
-        <v>3157</v>
+        <v>3156</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>124</v>
@@ -14251,7 +14281,7 @@
         <v>gfx/Fairy.gfx</v>
       </c>
       <c r="F103" t="s">
-        <v>3353</v>
+        <v>3350</v>
       </c>
       <c r="G103" s="5">
         <f t="shared" si="13"/>
@@ -14267,7 +14297,7 @@
     </row>
     <row r="104" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
-        <v>3398</v>
+        <v>3394</v>
       </c>
       <c r="C104" s="23" t="s">
         <v>51</v>
@@ -14291,7 +14321,7 @@
         <v>1</v>
       </c>
       <c r="M104" s="9" t="s">
-        <v>3265</v>
+        <v>3262</v>
       </c>
     </row>
     <row r="105" spans="1:20" x14ac:dyDescent="0.2">
@@ -14327,7 +14357,7 @@
         <v>15360</v>
       </c>
       <c r="R105" s="17" t="s">
-        <v>3268</v>
+        <v>3265</v>
       </c>
       <c r="T105" t="str">
         <f>RIGHT(R105,4)</f>
@@ -14367,7 +14397,7 @@
         <v>15408</v>
       </c>
       <c r="R106" s="17" t="s">
-        <v>3269</v>
+        <v>3266</v>
       </c>
       <c r="T106" t="str">
         <f t="shared" ref="T106:T117" si="22">RIGHT(R106,4)</f>
@@ -14407,7 +14437,7 @@
         <v>15456</v>
       </c>
       <c r="R107" s="17" t="s">
-        <v>3270</v>
+        <v>3267</v>
       </c>
       <c r="T107" t="str">
         <f t="shared" si="22"/>
@@ -14447,7 +14477,7 @@
         <v>16640</v>
       </c>
       <c r="R108" s="17" t="s">
-        <v>3271</v>
+        <v>3268</v>
       </c>
       <c r="T108" t="str">
         <f t="shared" si="22"/>
@@ -14487,7 +14517,7 @@
         <v>16688</v>
       </c>
       <c r="R109" s="17" t="s">
-        <v>3272</v>
+        <v>3269</v>
       </c>
       <c r="T109" t="str">
         <f t="shared" si="22"/>
@@ -14527,7 +14557,7 @@
         <v>20592</v>
       </c>
       <c r="R110" s="17" t="s">
-        <v>3273</v>
+        <v>3270</v>
       </c>
       <c r="T110" t="str">
         <f t="shared" si="22"/>
@@ -14567,7 +14597,7 @@
         <v>25856</v>
       </c>
       <c r="R111" s="17" t="s">
-        <v>3274</v>
+        <v>3271</v>
       </c>
       <c r="T111" t="str">
         <f t="shared" si="22"/>
@@ -14607,7 +14637,7 @@
         <v>25864</v>
       </c>
       <c r="R112" s="17" t="s">
-        <v>3275</v>
+        <v>3272</v>
       </c>
       <c r="T112" t="str">
         <f t="shared" si="22"/>
@@ -14647,7 +14677,7 @@
         <v>26560</v>
       </c>
       <c r="R113" s="17" t="s">
-        <v>3276</v>
+        <v>3273</v>
       </c>
       <c r="T113" t="str">
         <f t="shared" si="22"/>
@@ -14687,7 +14717,7 @@
         <v>26592</v>
       </c>
       <c r="R114" s="17" t="s">
-        <v>3277</v>
+        <v>3274</v>
       </c>
       <c r="T114" t="str">
         <f t="shared" si="22"/>
@@ -14727,7 +14757,7 @@
         <v>27232</v>
       </c>
       <c r="R115" s="17" t="s">
-        <v>3278</v>
+        <v>3275</v>
       </c>
       <c r="T115" t="str">
         <f t="shared" si="22"/>
@@ -14767,7 +14797,7 @@
         <v>30080</v>
       </c>
       <c r="R116" s="17" t="s">
-        <v>3279</v>
+        <v>3276</v>
       </c>
       <c r="T116" t="str">
         <f t="shared" si="22"/>
@@ -14807,7 +14837,7 @@
         <v>30344</v>
       </c>
       <c r="R117" s="17" t="s">
-        <v>3280</v>
+        <v>3277</v>
       </c>
       <c r="T117" t="str">
         <f t="shared" si="22"/>
@@ -14819,7 +14849,7 @@
         <v>212</v>
       </c>
       <c r="B118" t="s">
-        <v>3238</v>
+        <v>3235</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>124</v>
@@ -14851,7 +14881,7 @@
         <v>215</v>
       </c>
       <c r="B119" t="s">
-        <v>3237</v>
+        <v>3234</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>124</v>
@@ -14883,7 +14913,7 @@
         <v>218</v>
       </c>
       <c r="B120" t="s">
-        <v>3236</v>
+        <v>3233</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>124</v>
@@ -14915,7 +14945,7 @@
         <v>221</v>
       </c>
       <c r="B121" t="s">
-        <v>3330</v>
+        <v>3327</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>124</v>
@@ -14947,7 +14977,7 @@
         <v>224</v>
       </c>
       <c r="B122" t="s">
-        <v>3304</v>
+        <v>3301</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>124</v>
@@ -14979,7 +15009,7 @@
         <v>227</v>
       </c>
       <c r="B123" t="s">
-        <v>3305</v>
+        <v>3302</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>124</v>
@@ -15011,7 +15041,7 @@
         <v>230</v>
       </c>
       <c r="B124" t="s">
-        <v>3306</v>
+        <v>3303</v>
       </c>
       <c r="C124" s="5" t="s">
         <v>124</v>
@@ -15043,7 +15073,7 @@
         <v>233</v>
       </c>
       <c r="B125" t="s">
-        <v>3307</v>
+        <v>3304</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>124</v>
@@ -15075,7 +15105,7 @@
         <v>236</v>
       </c>
       <c r="B126" t="s">
-        <v>3308</v>
+        <v>3305</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>124</v>
@@ -15107,7 +15137,7 @@
         <v>239</v>
       </c>
       <c r="B127" t="s">
-        <v>3309</v>
+        <v>3306</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>124</v>
@@ -15139,7 +15169,7 @@
         <v>242</v>
       </c>
       <c r="B128" t="s">
-        <v>3310</v>
+        <v>3307</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>124</v>
@@ -15171,7 +15201,7 @@
         <v>245</v>
       </c>
       <c r="B129" t="s">
-        <v>3311</v>
+        <v>3308</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>124</v>
@@ -15203,7 +15233,7 @@
         <v>248</v>
       </c>
       <c r="B130" t="s">
-        <v>3312</v>
+        <v>3309</v>
       </c>
       <c r="C130" s="5" t="s">
         <v>124</v>
@@ -15235,7 +15265,7 @@
         <v>251</v>
       </c>
       <c r="B131" t="s">
-        <v>3313</v>
+        <v>3310</v>
       </c>
       <c r="C131" s="5" t="s">
         <v>124</v>
@@ -15267,7 +15297,7 @@
         <v>254</v>
       </c>
       <c r="B132" t="s">
-        <v>3314</v>
+        <v>3311</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>124</v>
@@ -15299,7 +15329,7 @@
         <v>257</v>
       </c>
       <c r="B133" t="s">
-        <v>3315</v>
+        <v>3312</v>
       </c>
       <c r="C133" s="5" t="s">
         <v>124</v>
@@ -15331,7 +15361,7 @@
         <v>260</v>
       </c>
       <c r="B134" t="s">
-        <v>3316</v>
+        <v>3313</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>124</v>
@@ -15363,7 +15393,7 @@
         <v>263</v>
       </c>
       <c r="B135" t="s">
-        <v>3317</v>
+        <v>3314</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>124</v>
@@ -15395,7 +15425,7 @@
         <v>266</v>
       </c>
       <c r="B136" t="s">
-        <v>3318</v>
+        <v>3315</v>
       </c>
       <c r="C136" s="5" t="s">
         <v>124</v>
@@ -15427,7 +15457,7 @@
         <v>269</v>
       </c>
       <c r="B137" t="s">
-        <v>3319</v>
+        <v>3316</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>124</v>
@@ -15459,7 +15489,7 @@
         <v>272</v>
       </c>
       <c r="B138" t="s">
-        <v>3320</v>
+        <v>3317</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>124</v>
@@ -15491,7 +15521,7 @@
         <v>275</v>
       </c>
       <c r="B139" t="s">
-        <v>3321</v>
+        <v>3318</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>124</v>
@@ -15523,7 +15553,7 @@
         <v>278</v>
       </c>
       <c r="B140" t="s">
-        <v>3322</v>
+        <v>3319</v>
       </c>
       <c r="C140" s="5" t="s">
         <v>124</v>
@@ -15555,7 +15585,7 @@
         <v>281</v>
       </c>
       <c r="B141" t="s">
-        <v>3323</v>
+        <v>3320</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>124</v>
@@ -15587,7 +15617,7 @@
         <v>284</v>
       </c>
       <c r="B142" t="s">
-        <v>3324</v>
+        <v>3321</v>
       </c>
       <c r="C142" s="5" t="s">
         <v>124</v>
@@ -15619,7 +15649,7 @@
         <v>287</v>
       </c>
       <c r="B143" t="s">
-        <v>3325</v>
+        <v>3322</v>
       </c>
       <c r="C143" s="5" t="s">
         <v>124</v>
@@ -15651,7 +15681,7 @@
         <v>290</v>
       </c>
       <c r="B144" t="s">
-        <v>3326</v>
+        <v>3323</v>
       </c>
       <c r="C144" s="5" t="s">
         <v>124</v>
@@ -15683,7 +15713,7 @@
         <v>293</v>
       </c>
       <c r="B145" t="s">
-        <v>3327</v>
+        <v>3324</v>
       </c>
       <c r="C145" s="5" t="s">
         <v>124</v>
@@ -15715,7 +15745,7 @@
         <v>296</v>
       </c>
       <c r="B146" t="s">
-        <v>3328</v>
+        <v>3325</v>
       </c>
       <c r="C146" s="5" t="s">
         <v>124</v>
@@ -15747,7 +15777,7 @@
         <v>298</v>
       </c>
       <c r="B147" t="s">
-        <v>3329</v>
+        <v>3326</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>124</v>
@@ -15760,7 +15790,7 @@
         <v>gfx/Main_Slots.offsets</v>
       </c>
       <c r="F147" t="s">
-        <v>3354</v>
+        <v>3351</v>
       </c>
       <c r="G147" s="5">
         <f t="shared" si="27"/>
@@ -15779,20 +15809,20 @@
         <v>299</v>
       </c>
       <c r="B148" t="s">
-        <v>3216</v>
+        <v>3215</v>
       </c>
       <c r="C148" s="5" t="s">
         <v>124</v>
       </c>
       <c r="D148" t="s">
-        <v>3217</v>
+        <v>3216</v>
       </c>
       <c r="E148" t="str">
         <f t="shared" si="26"/>
         <v>gfx/Switches.colours</v>
       </c>
       <c r="F148" t="s">
-        <v>3355</v>
+        <v>3352</v>
       </c>
       <c r="G148" s="5">
         <f t="shared" si="27"/>
@@ -15811,7 +15841,7 @@
         <v>300</v>
       </c>
       <c r="B149" t="s">
-        <v>3331</v>
+        <v>3328</v>
       </c>
       <c r="C149" s="5" t="s">
         <v>124</v>
@@ -15824,7 +15854,7 @@
         <v>gfx/Main_Sign.colours</v>
       </c>
       <c r="F149" t="s">
-        <v>3356</v>
+        <v>3353</v>
       </c>
       <c r="G149" s="5">
         <f t="shared" si="27"/>
@@ -15854,7 +15884,7 @@
         <v>3082</v>
       </c>
       <c r="B151" s="12" t="s">
-        <v>3183</v>
+        <v>3182</v>
       </c>
       <c r="C151" s="13"/>
       <c r="G151" s="13"/>
@@ -15866,7 +15896,7 @@
         <v>3089</v>
       </c>
       <c r="B152" t="s">
-        <v>3161</v>
+        <v>3160</v>
       </c>
       <c r="C152" s="7" t="s">
         <v>51</v>
@@ -15879,7 +15909,7 @@
         <v>monsters/Summon.gfx</v>
       </c>
       <c r="F152" t="s">
-        <v>3362</v>
+        <v>3359</v>
       </c>
       <c r="G152" s="5">
         <f t="shared" ref="G152:G158" si="29">IF(F152&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F152,"adrEA",""),"$","")),"")</f>
@@ -15894,7 +15924,7 @@
         <v>3090</v>
       </c>
       <c r="B153" t="s">
-        <v>3158</v>
+        <v>3157</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>51</v>
@@ -15907,7 +15937,7 @@
         <v>monsters/Behemoth.gfx</v>
       </c>
       <c r="F153" t="s">
-        <v>3363</v>
+        <v>3360</v>
       </c>
       <c r="G153" s="5">
         <f t="shared" si="29"/>
@@ -15930,7 +15960,7 @@
         <v>3091</v>
       </c>
       <c r="B154" t="s">
-        <v>3159</v>
+        <v>3158</v>
       </c>
       <c r="C154" s="7" t="s">
         <v>51</v>
@@ -15943,7 +15973,7 @@
         <v>monsters/Crab.gfx</v>
       </c>
       <c r="F154" t="s">
-        <v>3364</v>
+        <v>3361</v>
       </c>
       <c r="G154" s="5">
         <f t="shared" si="29"/>
@@ -15966,7 +15996,7 @@
         <v>3092</v>
       </c>
       <c r="B155" t="s">
-        <v>3160</v>
+        <v>3159</v>
       </c>
       <c r="C155" s="7" t="s">
         <v>51</v>
@@ -15979,7 +16009,7 @@
         <v>monsters/CrabClaw.gfx</v>
       </c>
       <c r="F155" t="s">
-        <v>3365</v>
+        <v>3362</v>
       </c>
       <c r="G155" s="5">
         <f t="shared" si="29"/>
@@ -16002,7 +16032,7 @@
         <v>2369</v>
       </c>
       <c r="B156" t="s">
-        <v>3162</v>
+        <v>3161</v>
       </c>
       <c r="C156" s="7" t="s">
         <v>51</v>
@@ -16024,7 +16054,7 @@
         <v>2370</v>
       </c>
       <c r="B157" t="s">
-        <v>3164</v>
+        <v>3163</v>
       </c>
       <c r="C157" s="7" t="s">
         <v>51</v>
@@ -16042,16 +16072,16 @@
         <v>3142</v>
       </c>
       <c r="B158" t="s">
-        <v>3163</v>
+        <v>3162</v>
       </c>
       <c r="C158" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E158" t="s">
-        <v>3367</v>
+        <v>3364</v>
       </c>
       <c r="F158" t="s">
-        <v>3366</v>
+        <v>3363</v>
       </c>
       <c r="G158" s="5">
         <f t="shared" si="29"/>
@@ -16071,16 +16101,16 @@
         <v>3133</v>
       </c>
       <c r="B159" t="s">
-        <v>3166</v>
+        <v>3165</v>
       </c>
       <c r="C159" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E159" t="s">
-        <v>3368</v>
+        <v>3365</v>
       </c>
       <c r="F159" t="s">
-        <v>3378</v>
+        <v>3375</v>
       </c>
       <c r="G159" s="5">
         <f t="shared" ref="G159:G167" si="30">IF(F159&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F159,"adrEA",""),"$","")),"")</f>
@@ -16108,16 +16138,16 @@
         <v>3134</v>
       </c>
       <c r="B160" t="s">
-        <v>3167</v>
+        <v>3166</v>
       </c>
       <c r="C160" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E160" t="s">
-        <v>3369</v>
+        <v>3366</v>
       </c>
       <c r="F160" t="s">
-        <v>3379</v>
+        <v>3376</v>
       </c>
       <c r="G160" s="5">
         <f t="shared" si="30"/>
@@ -16145,16 +16175,16 @@
         <v>3135</v>
       </c>
       <c r="B161" t="s">
-        <v>3168</v>
+        <v>3167</v>
       </c>
       <c r="C161" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E161" t="s">
-        <v>3370</v>
+        <v>3367</v>
       </c>
       <c r="F161" t="s">
-        <v>3380</v>
+        <v>3377</v>
       </c>
       <c r="G161" s="5">
         <f t="shared" si="30"/>
@@ -16182,16 +16212,16 @@
         <v>3136</v>
       </c>
       <c r="B162" t="s">
-        <v>3169</v>
+        <v>3168</v>
       </c>
       <c r="C162" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E162" t="s">
-        <v>3371</v>
+        <v>3368</v>
       </c>
       <c r="F162" t="s">
-        <v>3381</v>
+        <v>3378</v>
       </c>
       <c r="G162" s="5">
         <f t="shared" si="30"/>
@@ -16219,16 +16249,16 @@
         <v>3137</v>
       </c>
       <c r="B163" t="s">
-        <v>3170</v>
+        <v>3169</v>
       </c>
       <c r="C163" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E163" t="s">
-        <v>3372</v>
+        <v>3369</v>
       </c>
       <c r="F163" t="s">
-        <v>3382</v>
+        <v>3379</v>
       </c>
       <c r="G163" s="5">
         <f t="shared" si="30"/>
@@ -16256,16 +16286,16 @@
         <v>3138</v>
       </c>
       <c r="B164" t="s">
-        <v>3165</v>
+        <v>3164</v>
       </c>
       <c r="C164" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E164" t="s">
-        <v>3373</v>
+        <v>3370</v>
       </c>
       <c r="F164" t="s">
-        <v>3383</v>
+        <v>3380</v>
       </c>
       <c r="G164" s="5">
         <f t="shared" si="30"/>
@@ -16293,16 +16323,16 @@
         <v>3139</v>
       </c>
       <c r="B165" t="s">
-        <v>3171</v>
+        <v>3170</v>
       </c>
       <c r="C165" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E165" t="s">
-        <v>3374</v>
+        <v>3371</v>
       </c>
       <c r="F165" t="s">
-        <v>3384</v>
+        <v>3381</v>
       </c>
       <c r="G165" s="5">
         <f t="shared" si="30"/>
@@ -16330,16 +16360,16 @@
         <v>3140</v>
       </c>
       <c r="B166" t="s">
-        <v>3172</v>
+        <v>3171</v>
       </c>
       <c r="C166" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E166" t="s">
-        <v>3375</v>
+        <v>3372</v>
       </c>
       <c r="F166" t="s">
-        <v>3385</v>
+        <v>3382</v>
       </c>
       <c r="G166" s="5">
         <f t="shared" si="30"/>
@@ -16367,16 +16397,16 @@
         <v>3141</v>
       </c>
       <c r="B167" t="s">
-        <v>3173</v>
+        <v>3172</v>
       </c>
       <c r="C167" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E167" t="s">
-        <v>3376</v>
+        <v>3373</v>
       </c>
       <c r="F167" t="s">
-        <v>3386</v>
+        <v>3383</v>
       </c>
       <c r="G167" s="5">
         <f t="shared" si="30"/>
@@ -16404,7 +16434,7 @@
         <v>3093</v>
       </c>
       <c r="B168" t="s">
-        <v>3174</v>
+        <v>3173</v>
       </c>
       <c r="C168" s="7" t="s">
         <v>51</v>
@@ -16445,7 +16475,7 @@
         <v>3094</v>
       </c>
       <c r="B169" t="s">
-        <v>3175</v>
+        <v>3174</v>
       </c>
       <c r="C169" s="7" t="s">
         <v>51</v>
@@ -16486,7 +16516,7 @@
         <v>3095</v>
       </c>
       <c r="B170" t="s">
-        <v>3155</v>
+        <v>3154</v>
       </c>
       <c r="C170" s="5" t="s">
         <v>124</v>
@@ -16499,7 +16529,7 @@
         <v>gfx/Pockets.gfx</v>
       </c>
       <c r="F170" t="s">
-        <v>3282</v>
+        <v>3279</v>
       </c>
       <c r="G170" s="5">
         <f>IF(F170&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F170,"adrEA",""),"$","")),"")</f>
@@ -16521,13 +16551,13 @@
         <v>312190</v>
       </c>
       <c r="M170" t="s">
-        <v>3267</v>
+        <v>3264</v>
       </c>
       <c r="N170" s="21" t="s">
-        <v>3266</v>
+        <v>3263</v>
       </c>
       <c r="P170" t="s">
-        <v>3281</v>
+        <v>3278</v>
       </c>
       <c r="Q170" t="s">
         <v>3125</v>
@@ -16538,7 +16568,7 @@
         <v>3109</v>
       </c>
       <c r="B171" t="s">
-        <v>3176</v>
+        <v>3175</v>
       </c>
       <c r="C171" s="5" t="s">
         <v>195</v>
@@ -16575,34 +16605,34 @@
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>3181</v>
+        <v>3180</v>
       </c>
       <c r="B172" t="s">
-        <v>3183</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
+        <v>3181</v>
+      </c>
+      <c r="B173" t="s">
         <v>3182</v>
-      </c>
-      <c r="B173" t="s">
-        <v>3183</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>3184</v>
+        <v>3183</v>
       </c>
       <c r="B174" t="s">
-        <v>3183</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>3185</v>
+        <v>3184</v>
       </c>
       <c r="B175" t="s">
-        <v>3183</v>
+        <v>3182</v>
       </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
@@ -16610,7 +16640,7 @@
         <v>3110</v>
       </c>
       <c r="B176" t="s">
-        <v>3177</v>
+        <v>3176</v>
       </c>
       <c r="C176" s="5" t="s">
         <v>195</v>
@@ -16642,7 +16672,7 @@
         <v>3111</v>
       </c>
       <c r="B177" s="15" t="s">
-        <v>3178</v>
+        <v>3177</v>
       </c>
       <c r="C177" s="5" t="s">
         <v>195</v>
@@ -16674,7 +16704,7 @@
         <v>3112</v>
       </c>
       <c r="B178" s="15" t="s">
-        <v>3179</v>
+        <v>3178</v>
       </c>
       <c r="C178" s="5" t="s">
         <v>195</v>
@@ -16706,7 +16736,7 @@
         <v>3113</v>
       </c>
       <c r="B179" s="15" t="s">
-        <v>3180</v>
+        <v>3179</v>
       </c>
       <c r="C179" s="5" t="s">
         <v>195</v>
@@ -18435,20 +18465,20 @@
         <v>541</v>
       </c>
       <c r="B386" t="s">
-        <v>3394</v>
+        <v>3390</v>
       </c>
       <c r="C386" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D386" t="s">
-        <v>3396</v>
+        <v>3392</v>
       </c>
       <c r="E386" t="str">
         <f t="shared" ref="E386" si="39">C386&amp;"/"&amp;D386</f>
         <v>data/monsters.spellbook.block</v>
       </c>
       <c r="F386" t="s">
-        <v>3395</v>
+        <v>3391</v>
       </c>
       <c r="G386" s="5">
         <f t="shared" ref="G386" si="40">IF(F386&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F386,"adrEA",""),"$","")),"")</f>
@@ -22371,7 +22401,7 @@
         <v>1032</v>
       </c>
       <c r="B875" t="s">
-        <v>3223</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
@@ -22411,7 +22441,7 @@
         <v>1037</v>
       </c>
       <c r="B880" t="s">
-        <v>3224</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
@@ -25077,7 +25107,7 @@
         <v>1431</v>
       </c>
       <c r="B1214" t="s">
-        <v>3149</v>
+        <v>3148</v>
       </c>
     </row>
     <row r="1215" spans="1:2" x14ac:dyDescent="0.2">
@@ -25085,7 +25115,7 @@
         <v>1432</v>
       </c>
       <c r="B1215" t="s">
-        <v>3148</v>
+        <v>3147</v>
       </c>
     </row>
     <row r="1216" spans="1:2" x14ac:dyDescent="0.2">
@@ -25093,7 +25123,7 @@
         <v>1433</v>
       </c>
       <c r="B1216" t="s">
-        <v>3150</v>
+        <v>3149</v>
       </c>
     </row>
     <row r="1217" spans="1:2" x14ac:dyDescent="0.2">
@@ -25101,7 +25131,7 @@
         <v>1435</v>
       </c>
       <c r="B1217" t="s">
-        <v>3152</v>
+        <v>3151</v>
       </c>
     </row>
     <row r="1218" spans="1:2" x14ac:dyDescent="0.2">
@@ -25109,7 +25139,7 @@
         <v>1436</v>
       </c>
       <c r="B1218" t="s">
-        <v>3154</v>
+        <v>3153</v>
       </c>
     </row>
     <row r="1219" spans="1:2" x14ac:dyDescent="0.2">
@@ -25117,7 +25147,7 @@
         <v>1437</v>
       </c>
       <c r="B1219" t="s">
-        <v>3153</v>
+        <v>3152</v>
       </c>
     </row>
     <row r="1220" spans="1:2" x14ac:dyDescent="0.2">
@@ -25242,7 +25272,7 @@
         <v>1463</v>
       </c>
       <c r="B1235" t="s">
-        <v>3151</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="1236" spans="1:2" x14ac:dyDescent="0.2">
@@ -26274,7 +26304,7 @@
         <v>1599</v>
       </c>
       <c r="B1364" t="s">
-        <v>3225</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="1365" spans="1:2" x14ac:dyDescent="0.2">
@@ -26554,7 +26584,7 @@
         <v>1636</v>
       </c>
       <c r="B1399" t="s">
-        <v>3397</v>
+        <v>3393</v>
       </c>
       <c r="F1399">
         <v>16</v>
@@ -27487,7 +27517,7 @@
     </row>
     <row r="1516" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1516" t="s">
-        <v>3147</v>
+        <v>3146</v>
       </c>
       <c r="B1516" t="s">
         <v>1779</v>
@@ -27647,7 +27677,7 @@
         <v>1810</v>
       </c>
       <c r="B1536" t="s">
-        <v>3190</v>
+        <v>3189</v>
       </c>
     </row>
     <row r="1537" spans="1:2" x14ac:dyDescent="0.2">
@@ -27655,7 +27685,7 @@
         <v>1811</v>
       </c>
       <c r="B1537" t="s">
-        <v>3191</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="1538" spans="1:2" x14ac:dyDescent="0.2">
@@ -29687,7 +29717,7 @@
         <v>2080</v>
       </c>
       <c r="B1791" t="s">
-        <v>3284</v>
+        <v>3281</v>
       </c>
     </row>
     <row r="1792" spans="1:2" x14ac:dyDescent="0.2">
@@ -29695,7 +29725,7 @@
         <v>2081</v>
       </c>
       <c r="B1792" t="s">
-        <v>3283</v>
+        <v>3280</v>
       </c>
     </row>
     <row r="1793" spans="1:2" x14ac:dyDescent="0.2">
@@ -30457,7 +30487,7 @@
         <v>2182</v>
       </c>
       <c r="B1888" t="s">
-        <v>322</v>
+        <v>3411</v>
       </c>
     </row>
     <row r="1889" spans="1:2" x14ac:dyDescent="0.2">
@@ -30473,7 +30503,7 @@
         <v>2184</v>
       </c>
       <c r="B1890" t="s">
-        <v>322</v>
+        <v>3405</v>
       </c>
     </row>
     <row r="1891" spans="1:2" x14ac:dyDescent="0.2">
@@ -30489,7 +30519,7 @@
         <v>2186</v>
       </c>
       <c r="B1892" t="s">
-        <v>322</v>
+        <v>3412</v>
       </c>
     </row>
     <row r="1893" spans="1:2" x14ac:dyDescent="0.2">
@@ -30673,7 +30703,7 @@
         <v>2209</v>
       </c>
       <c r="B1915" t="s">
-        <v>3359</v>
+        <v>3356</v>
       </c>
     </row>
     <row r="1916" spans="1:3" x14ac:dyDescent="0.2">
@@ -30697,7 +30727,7 @@
         <v>2212</v>
       </c>
       <c r="C1918" s="5" t="s">
-        <v>3377</v>
+        <v>3374</v>
       </c>
     </row>
     <row r="1919" spans="1:3" x14ac:dyDescent="0.2">
@@ -31065,7 +31095,7 @@
         <v>322</v>
       </c>
       <c r="C1964" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1965" spans="1:3" x14ac:dyDescent="0.2">
@@ -31076,7 +31106,7 @@
         <v>322</v>
       </c>
       <c r="C1965" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1966" spans="1:3" x14ac:dyDescent="0.2">
@@ -31087,7 +31117,7 @@
         <v>322</v>
       </c>
       <c r="C1966" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1967" spans="1:3" x14ac:dyDescent="0.2">
@@ -31098,7 +31128,7 @@
         <v>322</v>
       </c>
       <c r="C1967" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1968" spans="1:3" x14ac:dyDescent="0.2">
@@ -31138,7 +31168,7 @@
         <v>322</v>
       </c>
       <c r="C1972" s="5" t="s">
-        <v>3189</v>
+        <v>3188</v>
       </c>
     </row>
     <row r="1973" spans="1:3" x14ac:dyDescent="0.2">
@@ -31181,7 +31211,7 @@
         <v>322</v>
       </c>
       <c r="C1977" s="5" t="s">
-        <v>3189</v>
+        <v>3188</v>
       </c>
     </row>
     <row r="1978" spans="1:3" x14ac:dyDescent="0.2">
@@ -31192,7 +31222,7 @@
         <v>322</v>
       </c>
       <c r="C1978" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1979" spans="1:3" x14ac:dyDescent="0.2">
@@ -31203,7 +31233,7 @@
         <v>322</v>
       </c>
       <c r="C1979" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1980" spans="1:3" x14ac:dyDescent="0.2">
@@ -31214,7 +31244,7 @@
         <v>322</v>
       </c>
       <c r="C1980" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1981" spans="1:3" x14ac:dyDescent="0.2">
@@ -31225,7 +31255,7 @@
         <v>322</v>
       </c>
       <c r="C1981" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1982" spans="1:3" x14ac:dyDescent="0.2">
@@ -31236,7 +31266,7 @@
         <v>322</v>
       </c>
       <c r="C1982" s="5" t="s">
-        <v>3188</v>
+        <v>3187</v>
       </c>
     </row>
     <row r="1983" spans="1:3" x14ac:dyDescent="0.2">
@@ -31268,7 +31298,7 @@
         <v>2290</v>
       </c>
       <c r="B1986" t="s">
-        <v>3400</v>
+        <v>3396</v>
       </c>
     </row>
     <row r="1987" spans="1:2" x14ac:dyDescent="0.2">
@@ -31276,7 +31306,7 @@
         <v>2291</v>
       </c>
       <c r="B1987" t="s">
-        <v>3401</v>
+        <v>3397</v>
       </c>
     </row>
     <row r="1988" spans="1:2" x14ac:dyDescent="0.2">
@@ -31484,7 +31514,7 @@
         <v>2319</v>
       </c>
       <c r="B2013" t="s">
-        <v>3407</v>
+        <v>3403</v>
       </c>
     </row>
     <row r="2014" spans="1:2" x14ac:dyDescent="0.2">
@@ -31492,7 +31522,7 @@
         <v>2320</v>
       </c>
       <c r="B2014" t="s">
-        <v>3408</v>
+        <v>3404</v>
       </c>
     </row>
     <row r="2015" spans="1:2" x14ac:dyDescent="0.2">
@@ -31889,7 +31919,7 @@
         <v>2375</v>
       </c>
       <c r="B2064" t="s">
-        <v>3357</v>
+        <v>3354</v>
       </c>
     </row>
     <row r="2065" spans="1:2" x14ac:dyDescent="0.2">
@@ -31897,7 +31927,7 @@
         <v>2376</v>
       </c>
       <c r="B2065" t="s">
-        <v>3358</v>
+        <v>3355</v>
       </c>
     </row>
     <row r="2066" spans="1:2" x14ac:dyDescent="0.2">
@@ -32190,10 +32220,10 @@
     </row>
     <row r="2102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2102" t="s">
-        <v>3404</v>
+        <v>3400</v>
       </c>
       <c r="B2102" t="s">
-        <v>3405</v>
+        <v>3401</v>
       </c>
       <c r="H2102" s="5">
         <v>24</v>
@@ -32208,7 +32238,7 @@
         <v>2418</v>
       </c>
       <c r="B2103" t="s">
-        <v>3403</v>
+        <v>3399</v>
       </c>
     </row>
     <row r="2104" spans="1:9" x14ac:dyDescent="0.2">
@@ -32216,7 +32246,7 @@
         <v>2419</v>
       </c>
       <c r="B2104" t="s">
-        <v>3406</v>
+        <v>3402</v>
       </c>
     </row>
     <row r="2105" spans="1:9" x14ac:dyDescent="0.2">
@@ -32291,7 +32321,7 @@
         <v>2430</v>
       </c>
       <c r="B2113" t="s">
-        <v>3187</v>
+        <v>3186</v>
       </c>
     </row>
     <row r="2114" spans="1:2" x14ac:dyDescent="0.2">
@@ -32987,7 +33017,7 @@
         <v>2519</v>
       </c>
       <c r="B2200" t="s">
-        <v>322</v>
+        <v>3414</v>
       </c>
     </row>
     <row r="2201" spans="1:2" x14ac:dyDescent="0.2">
@@ -33003,7 +33033,7 @@
         <v>2521</v>
       </c>
       <c r="B2202" t="s">
-        <v>322</v>
+        <v>3416</v>
       </c>
     </row>
     <row r="2203" spans="1:2" x14ac:dyDescent="0.2">
@@ -33019,7 +33049,7 @@
         <v>2523</v>
       </c>
       <c r="B2204" t="s">
-        <v>322</v>
+        <v>3418</v>
       </c>
     </row>
     <row r="2205" spans="1:2" x14ac:dyDescent="0.2">
@@ -33035,7 +33065,7 @@
         <v>2525</v>
       </c>
       <c r="B2206" t="s">
-        <v>322</v>
+        <v>3417</v>
       </c>
     </row>
     <row r="2207" spans="1:2" x14ac:dyDescent="0.2">
@@ -33107,7 +33137,7 @@
         <v>2534</v>
       </c>
       <c r="B2215" t="s">
-        <v>322</v>
+        <v>3415</v>
       </c>
     </row>
     <row r="2216" spans="1:9" x14ac:dyDescent="0.2">
@@ -33123,7 +33153,7 @@
         <v>2536</v>
       </c>
       <c r="B2217" t="s">
-        <v>3339</v>
+        <v>3336</v>
       </c>
       <c r="C2217" s="5" t="s">
         <v>124</v>
@@ -33136,7 +33166,7 @@
         <v>gfx/Main_Slots.colours</v>
       </c>
       <c r="F2217" t="s">
-        <v>3338</v>
+        <v>3335</v>
       </c>
       <c r="G2217" s="5">
         <f t="shared" ref="G2217" si="44">IF(F2217&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F2217,"adrEA",""),"$","")),"")</f>
@@ -33163,7 +33193,7 @@
         <v>2538</v>
       </c>
       <c r="B2219" t="s">
-        <v>322</v>
+        <v>3413</v>
       </c>
     </row>
     <row r="2220" spans="1:9" x14ac:dyDescent="0.2">
@@ -33171,20 +33201,20 @@
         <v>2539</v>
       </c>
       <c r="B2220" t="s">
-        <v>3388</v>
+        <v>3384</v>
       </c>
       <c r="C2220" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D2220" t="s">
-        <v>3389</v>
+        <v>3385</v>
       </c>
       <c r="E2220" t="str">
         <f t="shared" ref="E2220" si="46">C2220&amp;"/"&amp;D2220</f>
         <v>data/Door_Lock.colours</v>
       </c>
       <c r="F2220" t="s">
-        <v>3390</v>
+        <v>3386</v>
       </c>
       <c r="G2220" s="5">
         <f t="shared" ref="G2220" si="47">IF(F2220&lt;&gt;"",HEX2DEC(SUBSTITUTE(SUBSTITUTE(F2220,"adrEA",""),"$","")),"")</f>
@@ -33315,7 +33345,7 @@
         <v>2554</v>
       </c>
       <c r="B2235" t="s">
-        <v>322</v>
+        <v>3410</v>
       </c>
     </row>
     <row r="2236" spans="1:2" x14ac:dyDescent="0.2">
@@ -33355,7 +33385,7 @@
         <v>2559</v>
       </c>
       <c r="B2240" t="s">
-        <v>3361</v>
+        <v>3358</v>
       </c>
     </row>
     <row r="2241" spans="1:2" x14ac:dyDescent="0.2">
@@ -33363,7 +33393,7 @@
         <v>2560</v>
       </c>
       <c r="B2241" t="s">
-        <v>3360</v>
+        <v>3357</v>
       </c>
     </row>
     <row r="2242" spans="1:2" x14ac:dyDescent="0.2">
@@ -33371,7 +33401,7 @@
         <v>2561</v>
       </c>
       <c r="B2242" t="s">
-        <v>3391</v>
+        <v>3387</v>
       </c>
     </row>
     <row r="2243" spans="1:2" x14ac:dyDescent="0.2">
@@ -35716,7 +35746,7 @@
         <v>2917</v>
       </c>
       <c r="B2540" t="s">
-        <v>3226</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="2541" spans="1:2" x14ac:dyDescent="0.2">
@@ -35724,7 +35754,7 @@
         <v>2918</v>
       </c>
       <c r="B2541" t="s">
-        <v>3227</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="2542" spans="1:2" x14ac:dyDescent="0.2">
@@ -35809,7 +35839,7 @@
         <v>2936</v>
       </c>
       <c r="B2552" t="s">
-        <v>3221</v>
+        <v>3218</v>
       </c>
     </row>
     <row r="2553" spans="1:2" x14ac:dyDescent="0.2">
@@ -35833,7 +35863,7 @@
         <v>2941</v>
       </c>
       <c r="B2555" s="9" t="s">
-        <v>3219</v>
+        <v>3406</v>
       </c>
     </row>
     <row r="2556" spans="1:2" x14ac:dyDescent="0.2">
@@ -35841,7 +35871,7 @@
         <v>2942</v>
       </c>
       <c r="B2556" s="9" t="s">
-        <v>3218</v>
+        <v>3407</v>
       </c>
     </row>
     <row r="2557" spans="1:2" x14ac:dyDescent="0.2">
@@ -35849,7 +35879,7 @@
         <v>2943</v>
       </c>
       <c r="B2557" s="9" t="s">
-        <v>3387</v>
+        <v>3408</v>
       </c>
     </row>
     <row r="2558" spans="1:2" x14ac:dyDescent="0.2">
@@ -35857,7 +35887,7 @@
         <v>2945</v>
       </c>
       <c r="B2558" t="s">
-        <v>3145</v>
+        <v>3409</v>
       </c>
     </row>
     <row r="2559" spans="1:2" x14ac:dyDescent="0.2">
@@ -35881,7 +35911,7 @@
         <v>2948</v>
       </c>
       <c r="B2561" t="s">
-        <v>3285</v>
+        <v>3282</v>
       </c>
     </row>
     <row r="2562" spans="1:2" x14ac:dyDescent="0.2">
@@ -35897,7 +35927,7 @@
         <v>2950</v>
       </c>
       <c r="B2563" t="s">
-        <v>3220</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="2564" spans="1:2" x14ac:dyDescent="0.2">
@@ -36094,7 +36124,7 @@
         <v>2976</v>
       </c>
       <c r="B2588" t="s">
-        <v>3286</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="2589" spans="1:2" x14ac:dyDescent="0.2">
@@ -36118,7 +36148,7 @@
         <v>2979</v>
       </c>
       <c r="B2591" t="s">
-        <v>3288</v>
+        <v>3285</v>
       </c>
     </row>
     <row r="2592" spans="1:2" x14ac:dyDescent="0.2">
@@ -36222,7 +36252,7 @@
         <v>2992</v>
       </c>
       <c r="B2604" t="s">
-        <v>3287</v>
+        <v>3284</v>
       </c>
     </row>
     <row r="2605" spans="1:2" x14ac:dyDescent="0.2">
@@ -36238,7 +36268,7 @@
         <v>2994</v>
       </c>
       <c r="B2606" t="s">
-        <v>3289</v>
+        <v>3286</v>
       </c>
     </row>
     <row r="2607" spans="1:2" x14ac:dyDescent="0.2">
@@ -36355,7 +36385,7 @@
         <v>3019</v>
       </c>
       <c r="B2620" t="s">
-        <v>3402</v>
+        <v>3398</v>
       </c>
       <c r="H2620" s="5">
         <f>16*8*4</f>
@@ -36461,7 +36491,7 @@
         <v>3035</v>
       </c>
       <c r="B2633" t="s">
-        <v>3222</v>
+        <v>3219</v>
       </c>
     </row>
     <row r="2634" spans="1:2" x14ac:dyDescent="0.2">
@@ -36525,7 +36555,7 @@
         <v>3043</v>
       </c>
       <c r="B2641" t="s">
-        <v>3146</v>
+        <v>3145</v>
       </c>
     </row>
     <row r="2642" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Some extra data tables identified and monster attacks lookup table
</commit_message>
<xml_diff>
--- a/segments.xlsx
+++ b/segments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom.cresswell/Dropbox/Geek/Gaming Projects/Bloodwych 68k/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614A19D8-A467-884D-8E3E-38735BC16714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808B928A-F928-7842-BF02-7E23579EF903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="880" windowWidth="32720" windowHeight="22140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3280" yWindow="880" windowWidth="32720" windowHeight="22140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOODWYCH439" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BLOODWYCH439!$A$1:$M$2644</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5765" uniqueCount="3419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5765" uniqueCount="3428">
   <si>
     <t>Type</t>
   </si>
@@ -10293,6 +10293,33 @@
   </si>
   <si>
     <t>Draw_Main_Switch_Overlay</t>
+  </si>
+  <si>
+    <t>MonsterAttackTypeTable</t>
+  </si>
+  <si>
+    <t>AttackType_NoSpells</t>
+  </si>
+  <si>
+    <t>AttackType_Spells</t>
+  </si>
+  <si>
+    <t>AttackType_Drone</t>
+  </si>
+  <si>
+    <t>AttackType_DroneSpells</t>
+  </si>
+  <si>
+    <t>AttackType_ArcBoltMachine</t>
+  </si>
+  <si>
+    <t>Monster_Movement_DataTable</t>
+  </si>
+  <si>
+    <t>DroppedObjects_DataTable</t>
+  </si>
+  <si>
+    <t>.DropTheObject</t>
   </si>
 </sst>
 </file>
@@ -10847,8 +10874,8 @@
   <dimension ref="A1:T2644"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A2187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2216" sqref="D2216"/>
+      <pane ySplit="3" topLeftCell="A516" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C537" sqref="C537"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18449,7 +18476,7 @@
         <v>539</v>
       </c>
       <c r="B384" t="s">
-        <v>322</v>
+        <v>3419</v>
       </c>
     </row>
     <row r="385" spans="1:9" x14ac:dyDescent="0.2">
@@ -18457,7 +18484,7 @@
         <v>540</v>
       </c>
       <c r="B385" t="s">
-        <v>322</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="386" spans="1:9" x14ac:dyDescent="0.2">
@@ -18497,7 +18524,7 @@
         <v>542</v>
       </c>
       <c r="B387" t="s">
-        <v>322</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="388" spans="1:9" x14ac:dyDescent="0.2">
@@ -18537,7 +18564,7 @@
         <v>547</v>
       </c>
       <c r="B392" t="s">
-        <v>322</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="393" spans="1:9" x14ac:dyDescent="0.2">
@@ -18545,7 +18572,7 @@
         <v>548</v>
       </c>
       <c r="B393" t="s">
-        <v>322</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="394" spans="1:9" x14ac:dyDescent="0.2">
@@ -18609,7 +18636,7 @@
         <v>556</v>
       </c>
       <c r="B401" t="s">
-        <v>322</v>
+        <v>3422</v>
       </c>
     </row>
     <row r="402" spans="1:2" x14ac:dyDescent="0.2">
@@ -18673,7 +18700,7 @@
         <v>564</v>
       </c>
       <c r="B409" t="s">
-        <v>322</v>
+        <v>3425</v>
       </c>
     </row>
     <row r="410" spans="1:2" x14ac:dyDescent="0.2">
@@ -19753,7 +19780,7 @@
         <v>699</v>
       </c>
       <c r="B544" t="s">
-        <v>322</v>
+        <v>3427</v>
       </c>
     </row>
     <row r="545" spans="1:2" x14ac:dyDescent="0.2">
@@ -19761,7 +19788,7 @@
         <v>700</v>
       </c>
       <c r="B545" t="s">
-        <v>322</v>
+        <v>3426</v>
       </c>
     </row>
     <row r="546" spans="1:2" x14ac:dyDescent="0.2">
@@ -36611,7 +36638,7 @@
       <formula>MATCH(A2,A:A,0)&lt;&gt;ROW(A2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B74 A75:A77 A78:B147 A150:B176 A177:A179 A2432:A2460 A2461:B2476 A2477:A2505 A2506:B2515 A2516:A2532 A2533:B2543 A2544:A2547 A2548:B2554 A2555:A2567 A2568:B2580 A2581:A2604 A2605:B2620 A2621:A2627 A2628:B1048576 B1 H1:I151 B76:B77 B148:B149 H152:H157 I152:I168 H168 B2432:B2459 B2477:B2504 B2516:B2531 B2544:B2546 B2558:B2566 B2581:B2603 B2621:B2626 H169:I1048576 A180:B2431">
+  <conditionalFormatting sqref="A2:B74 A75:A77 A78:B147 A150:B176 A177:A179 A180:B2431 A2432:A2460 A2461:B2476 A2477:A2505 A2506:B2515 A2516:A2532 A2533:B2543 A2544:A2547 A2548:B2554 A2555:A2567 A2568:B2580 A2581:A2604 A2605:B2620 A2621:A2627 A2628:B1048576 B1 H1:I151 B76:B77 B148:B149 H152:H157 I152:I168 H168 H169:I1048576 B2432:B2459 B2477:B2504 B2516:B2531 B2544:B2546 B2558:B2566 B2581:B2603 B2621:B2626">
     <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
       <formula>AND(A1&lt;&gt;"",_xlfn.ISFORMULA(A1)=TRUE)</formula>
     </cfRule>

</xml_diff>

<commit_message>
some trader sections identified
</commit_message>
<xml_diff>
--- a/segments.xlsx
+++ b/segments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dom.cresswell/Dropbox/Geek/Gaming Projects/Bloodwych 68k/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808B928A-F928-7842-BF02-7E23579EF903}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E1323E9-5BCC-D24C-98A8-664CFF567194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3280" yWindow="880" windowWidth="32720" windowHeight="22140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12620" yWindow="1240" windowWidth="32720" windowHeight="22140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BLOODWYCH439" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5765" uniqueCount="3428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5765" uniqueCount="3432">
   <si>
     <t>Type</t>
   </si>
@@ -10320,6 +10320,18 @@
   </si>
   <si>
     <t>.DropTheObject</t>
+  </si>
+  <si>
+    <t>.Trader_NotPotionsButArms</t>
+  </si>
+  <si>
+    <t>ArmouryList</t>
+  </si>
+  <si>
+    <t>Trade_Exchange_TBC</t>
+  </si>
+  <si>
+    <t>Trade_Offer_TBC</t>
   </si>
 </sst>
 </file>
@@ -10874,8 +10886,8 @@
   <dimension ref="A1:T2644"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A516" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C537" sqref="C537"/>
+      <pane ySplit="3" topLeftCell="A677" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B704" sqref="B704"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20924,7 +20936,7 @@
         <v>843</v>
       </c>
       <c r="B687" t="s">
-        <v>322</v>
+        <v>3430</v>
       </c>
     </row>
     <row r="688" spans="1:2" x14ac:dyDescent="0.2">
@@ -21164,7 +21176,7 @@
         <v>873</v>
       </c>
       <c r="B717" t="s">
-        <v>322</v>
+        <v>3429</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.2">
@@ -21180,7 +21192,7 @@
         <v>875</v>
       </c>
       <c r="B719" t="s">
-        <v>322</v>
+        <v>3431</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.2">
@@ -21196,7 +21208,7 @@
         <v>877</v>
       </c>
       <c r="B721" t="s">
-        <v>322</v>
+        <v>3428</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.2">
@@ -36638,7 +36650,7 @@
       <formula>MATCH(A2,A:A,0)&lt;&gt;ROW(A2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:B74 A75:A77 A78:B147 A150:B176 A177:A179 A180:B2431 A2432:A2460 A2461:B2476 A2477:A2505 A2506:B2515 A2516:A2532 A2533:B2543 A2544:A2547 A2548:B2554 A2555:A2567 A2568:B2580 A2581:A2604 A2605:B2620 A2621:A2627 A2628:B1048576 B1 H1:I151 B76:B77 B148:B149 H152:H157 I152:I168 H168 H169:I1048576 B2432:B2459 B2477:B2504 B2516:B2531 B2544:B2546 B2558:B2566 B2581:B2603 B2621:B2626">
+  <conditionalFormatting sqref="A2:B74 A75:A77 A78:B147 A150:B176 A177:A179 A2432:A2460 A2461:B2476 A2477:A2505 A2506:B2515 A2516:A2532 A2533:B2543 A2544:A2547 A2548:B2554 A2555:A2567 A2568:B2580 A2581:A2604 A2605:B2620 A2621:A2627 A2628:B1048576 B1 H1:I151 B76:B77 B148:B149 H152:H157 I152:I168 H168 H169:I1048576 B2432:B2459 B2477:B2504 B2516:B2531 B2544:B2546 B2558:B2566 B2581:B2603 B2621:B2626 A180:B2431">
     <cfRule type="expression" dxfId="1" priority="11" stopIfTrue="1">
       <formula>AND(A1&lt;&gt;"",_xlfn.ISFORMULA(A1)=TRUE)</formula>
     </cfRule>

</xml_diff>